<commit_message>
added lme designations to orphans
</commit_message>
<xml_diff>
--- a/data/orphans.xlsx
+++ b/data/orphans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairegonzales/Documents/R projects/Chapter_1_research/sythesis_colocation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048F302D-7500-DE4E-8B82-00E43314BD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A16CE3-8DEB-1848-B11A-3A6CB6429362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="500" windowWidth="27240" windowHeight="15920" xr2:uid="{9B0CDDD0-159A-4B47-8720-92FCED52F2E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
   <si>
     <t>first_author</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Michler-Cieluch and Krause</t>
   </si>
   <si>
-    <t>Reflections on integrating operation and maintenance activities of offshore wind farms and maricultur</t>
-  </si>
-  <si>
     <t>Banach</t>
   </si>
   <si>
@@ -284,9 +281,6 @@
     <t>url</t>
   </si>
   <si>
-    <t>Ecology</t>
-  </si>
-  <si>
     <t>governance</t>
   </si>
   <si>
@@ -297,6 +291,33 @@
   </si>
   <si>
     <t>These are going to be reintegrated into the count data BUT we need to go back through and make sure these are in fact orpahns. Aka do they fall into ecology socio econ or governance and maybe we just missed that the first time around?</t>
+  </si>
+  <si>
+    <t>Reflections on integrating operation and maintenance activities of offshore wind farms and mariculture</t>
+  </si>
+  <si>
+    <t>lme</t>
+  </si>
+  <si>
+    <t>North Sea</t>
+  </si>
+  <si>
+    <t>Mediterranean Sea</t>
+  </si>
+  <si>
+    <t>ecology</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>NE U.S. Continental Shelf</t>
+  </si>
+  <si>
+    <t>Celtic-Biscay Shelf</t>
   </si>
 </sst>
 </file>
@@ -326,12 +347,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -347,10 +374,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -666,466 +707,578 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2897094-E271-7143-94AB-A3D835E09D85}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="1">
         <v>2009</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1">
         <v>2011</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="B4" s="1">
         <v>2013</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>2014</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="1">
         <v>2014</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E6" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="1">
         <v>2014</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="1">
         <v>2015</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>2015</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E9" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>2015</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>2015</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="1">
         <v>2016</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="43" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>2016</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="1">
         <v>2016</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2017</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="6"/>
+      <c r="I15" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1">
         <v>2017</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="1">
         <v>2017</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="1">
         <v>2017</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1">
         <v>2017</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="1">
         <v>2017</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="1">
         <v>2017</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="1">
         <v>2017</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1">
         <v>2017</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="1">
         <v>2018</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="1">
         <v>2018</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="1">
         <v>2019</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>2019</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1">
         <v>2019</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="43" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="1">
         <v>2019</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" s="1">
         <v>2019</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1">
         <v>2019</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1">
         <v>2020</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1">
         <v>2020</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="1">
         <v>2020</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="1">
         <v>2020</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="E35" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="6">
         <v>2020</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B37" s="1">
         <v>2020</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>80</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H37">
     <sortCondition ref="B2:B37"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D37" r:id="rId1" xr:uid="{20A1A908-0288-2C42-A423-A54DEAB88812}"/>
+    <hyperlink ref="I37" r:id="rId1" xr:uid="{20A1A908-0288-2C42-A423-A54DEAB88812}"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://celebrating200years.noaa.gov/breakthroughs/ecosystems/sup_lmes_map.html" xr:uid="{9D5C378D-DDD2-AE43-BDC9-1C12256D30EE}"/>
+    <hyperlink ref="E20" r:id="rId3" display="https://celebrating200years.noaa.gov/breakthroughs/ecosystems/sup_lmes_map.html" xr:uid="{D7CD7CB9-B65E-3247-8178-92A8F01C050A}"/>
+    <hyperlink ref="E24" r:id="rId4" display="https://celebrating200years.noaa.gov/breakthroughs/ecosystems/sup_lmes_map.html" xr:uid="{572B69A2-7C58-524F-A085-F63526981876}"/>
+    <hyperlink ref="E26" r:id="rId5" display="https://celebrating200years.noaa.gov/breakthroughs/ecosystems/sup_lmes_map.html" xr:uid="{E82475D5-3702-054E-8F98-3C63D35E5660}"/>
+    <hyperlink ref="C27" r:id="rId6" xr:uid="{43B59096-9807-B047-BCD6-53B2A88D3851}"/>
+    <hyperlink ref="I29" r:id="rId7" xr:uid="{287DFC3E-9375-9D47-AB7A-C040D5F8CB23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1143,12 +1296,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>